<commit_message>
Excel sheets prepared and PFDs exported with data for highly-detailed vector images.
</commit_message>
<xml_diff>
--- a/results/IRIS-distribution.xlsx
+++ b/results/IRIS-distribution.xlsx
@@ -8,46 +8,68 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rovin\Development\C++\College\Racunalna Inteligencija\Seminar\neural-networks-partical-swarm-optimization\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CF74D90-38F9-4426-98B7-2639E5F0B9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79BE929-2606-42F8-A86C-36D3147C2B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEC1424F-8C97-4D0A-A941-5A2A0CB526D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E244C25E-E3CB-48AB-B7AD-0D5421FCE116}"/>
   </bookViews>
   <sheets>
     <sheet name="IRIS-distribution" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
-    <t>TestRun</t>
+    <t>Iteracija</t>
   </si>
   <si>
-    <t>NumCorrect</t>
+    <t>Točno</t>
   </si>
   <si>
-    <t>NumWrong</t>
+    <t>Krivo</t>
   </si>
   <si>
-    <t>Train(0)OrTest(1)</t>
+    <t>Treniranje</t>
   </si>
   <si>
-    <t>AvgSuccess</t>
+    <t>Testiranje</t>
   </si>
   <si>
-    <t>AvgFailure</t>
+    <t>Σ Iteracija</t>
   </si>
   <si>
-    <t>Σ Accuracy</t>
+    <t>Prosjek točno</t>
+  </si>
+  <si>
+    <t>Prosjek krivo</t>
+  </si>
+  <si>
+    <t>Točnost rezultata (%)</t>
+  </si>
+  <si>
+    <t>Σ Pogodaka po iteraciji</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +198,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
@@ -524,24 +555,34 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="35" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="36" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="0" xfId="34" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="23" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="35" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="36" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="34" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="35"/>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" xfId="34" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -634,10 +675,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="hr-HR"/>
-              <a:t>Testing  threads</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Treniranje</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -674,19 +714,19 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IRIS-distribution'!$B$1</c:f>
+              <c:f>'IRIS-distribution'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NumCorrect</c:v>
+                  <c:v>Točno</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -701,87 +741,273 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'IRIS-distribution'!$A$12:$A$21</c:f>
+              <c:f>'IRIS-distribution'!$B$3:$B$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'IRIS-distribution'!$B$12:$B$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BB1B-4222-9282-60DBF9070E02}"/>
+              <c16:uniqueId val="{00000000-1D7F-4B1F-B060-CD85F2DC9C34}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -790,11 +1016,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IRIS-distribution'!$C$1</c:f>
+              <c:f>'IRIS-distribution'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NumWrong</c:v>
+                  <c:v>Krivo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -809,87 +1035,273 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'IRIS-distribution'!$A$12:$A$21</c:f>
+              <c:f>'IRIS-distribution'!$C$3:$C$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="54">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="55">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="61">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="69">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="76">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="77">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="79">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="80">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="83">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'IRIS-distribution'!$C$12:$C$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13</c:v>
+                <c:pt idx="84">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BB1B-4222-9282-60DBF9070E02}"/>
+              <c16:uniqueId val="{00000001-1D7F-4B1F-B060-CD85F2DC9C34}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -903,17 +1315,16 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1471887183"/>
-        <c:axId val="1471897743"/>
+        <c:axId val="2133963903"/>
+        <c:axId val="2133965823"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1471887183"/>
+        <c:axId val="2133963903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -950,7 +1361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1471897743"/>
+        <c:crossAx val="2133965823"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -958,12 +1369,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1471897743"/>
+        <c:axId val="2133965823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -978,7 +1389,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1009,7 +1420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1471887183"/>
+        <c:crossAx val="2133963903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,6 +1465,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1123,8 +1541,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="hr-HR"/>
-              <a:t>Training threads</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Testiranje</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1162,19 +1580,19 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IRIS-distribution'!$B$1</c:f>
+              <c:f>'IRIS-distribution'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NumCorrect</c:v>
+                  <c:v>Točno</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1191,46 +1609,298 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'IRIS-distribution'!$B$2:$B$11</c:f>
+              <c:f>'IRIS-distribution'!$E$3:$E$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>62</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59</c:v>
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2708-4839-B7B1-CE393DB87980}"/>
+              <c16:uniqueId val="{00000000-21F1-40C1-B11E-596578876AC0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1239,11 +1909,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'IRIS-distribution'!$C$1</c:f>
+              <c:f>'IRIS-distribution'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NumWrong</c:v>
+                  <c:v>Krivo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1260,46 +1930,298 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'IRIS-distribution'!$C$2:$C$11</c:f>
+              <c:f>'IRIS-distribution'!$F$3:$F$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="102"/>
                 <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="21">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="38">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="45">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="75">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="83">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
+                <c:pt idx="84">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-2708-4839-B7B1-CE393DB87980}"/>
+              <c16:uniqueId val="{00000001-21F1-40C1-B11E-596578876AC0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1313,17 +2235,16 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1471887183"/>
-        <c:axId val="1471897743"/>
+        <c:axId val="2133963903"/>
+        <c:axId val="2133965823"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1471887183"/>
+        <c:axId val="2133963903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1360,7 +2281,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1471897743"/>
+        <c:crossAx val="2133965823"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1368,12 +2289,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1471897743"/>
+        <c:axId val="2133965823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1388,7 +2309,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1419,7 +2340,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1471887183"/>
+        <c:crossAx val="2133963903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1464,6 +2385,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2593,23 +3521,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>256761</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>48930</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6348</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>35378</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>320692</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>2509</xdr:rowOff>
+      <xdr:colOff>827312</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F43DABE9-3FF2-C2D7-F806-F11474DD394D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1112E66-9B4D-B350-70FC-C1F862C12278}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2629,23 +3557,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>255804</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>170430</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5953</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>319735</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>124009</xdr:rowOff>
+      <xdr:colOff>826745</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>6463</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEE2AE0A-8FB9-4EC9-8235-D1CADB1BA323}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{382A1438-B7F8-4DE6-A092-E6961301D543}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2984,709 +3912,2050 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECDA8B1E-2C89-4911-A5A0-0D2CE756F1CC}">
-  <dimension ref="A1:P21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CE46D7-7FDA-4345-A5EE-4A67970D1318}">
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="H1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>78</v>
+      </c>
+      <c r="F3" s="9">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1">
+        <f>MAX(A$3:A$104)</f>
+        <v>100</v>
+      </c>
+      <c r="I3" s="1">
+        <f>SUM(B$3:B$104)/$H$3</f>
+        <v>77.59</v>
+      </c>
+      <c r="J3" s="1">
+        <f>SUM(C$3:C$104)/$H$3</f>
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1">
+        <v>27</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>73</v>
+      </c>
+      <c r="F4" s="9">
+        <v>32</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="1">
+        <f>SUM(B$3:C$3)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="B5" s="1">
+        <v>83</v>
+      </c>
+      <c r="C5" s="1">
+        <v>19</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9">
+        <v>82</v>
+      </c>
+      <c r="F5" s="9">
+        <v>23</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="1">
+        <f>ROUND(I$3/J$4,4) * 100</f>
+        <v>76.070000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="B6" s="1">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>96</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="B7" s="1">
+        <v>91</v>
+      </c>
+      <c r="C7" s="1">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>94</v>
+      </c>
+      <c r="F7" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>93</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9">
+        <v>6</v>
+      </c>
+      <c r="E8" s="9">
+        <v>89</v>
+      </c>
+      <c r="F8" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>94</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9">
+        <v>90</v>
+      </c>
+      <c r="F9" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>75</v>
+      </c>
+      <c r="C10" s="1">
+        <v>27</v>
+      </c>
+      <c r="D10" s="9">
+        <v>9</v>
+      </c>
+      <c r="E10" s="9">
+        <v>95</v>
+      </c>
+      <c r="F10" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>98</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>10</v>
+      </c>
+      <c r="E11" s="9">
+        <v>84</v>
+      </c>
+      <c r="F11" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>90</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" s="9">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9">
+        <v>93</v>
+      </c>
+      <c r="F12" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>90</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="9">
+        <v>12</v>
+      </c>
+      <c r="E13" s="9">
+        <v>91</v>
+      </c>
+      <c r="F13" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9">
+        <v>13</v>
+      </c>
+      <c r="E14" s="9">
+        <v>88</v>
+      </c>
+      <c r="F14" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9">
+        <v>14</v>
+      </c>
+      <c r="E15" s="9">
+        <v>90</v>
+      </c>
+      <c r="F15" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9</v>
+      </c>
+      <c r="D16" s="9">
+        <v>15</v>
+      </c>
+      <c r="E16" s="9">
+        <v>78</v>
+      </c>
+      <c r="F16" s="9">
+        <v>27</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="9">
+        <v>16</v>
+      </c>
+      <c r="E17" s="9">
+        <v>97</v>
+      </c>
+      <c r="F17" s="9">
+        <v>8</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>95</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7</v>
+      </c>
+      <c r="D18" s="9">
+        <v>19</v>
+      </c>
+      <c r="E18" s="9">
+        <v>89</v>
+      </c>
+      <c r="F18" s="9">
+        <v>16</v>
+      </c>
+      <c r="H18" s="9">
+        <f>MAX(D$3:D$104)</f>
+        <v>100</v>
+      </c>
+      <c r="I18" s="9">
+        <f>SUM(E$3:E$104)/$H$18</f>
+        <v>85.13</v>
+      </c>
+      <c r="J18" s="9">
+        <f>SUM(F$3:F$104)/$H$18</f>
+        <v>13.57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>91</v>
+      </c>
+      <c r="C19" s="1">
+        <v>11</v>
+      </c>
+      <c r="D19" s="9">
+        <v>20</v>
+      </c>
+      <c r="E19" s="9">
+        <v>92</v>
+      </c>
+      <c r="F19" s="9">
+        <v>13</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="9">
+        <f>SUM(E$3:F$3)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>91</v>
+      </c>
+      <c r="C20" s="1">
+        <v>11</v>
+      </c>
+      <c r="D20" s="9">
+        <v>21</v>
+      </c>
+      <c r="E20" s="9">
+        <v>97</v>
+      </c>
+      <c r="F20" s="9">
+        <v>8</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="9">
+        <f>ROUND(I$18/J$19,4) * 100</f>
+        <v>81.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>91</v>
+      </c>
+      <c r="C21" s="1">
+        <v>11</v>
+      </c>
+      <c r="D21" s="9">
+        <v>22</v>
+      </c>
+      <c r="E21" s="9">
+        <v>88</v>
+      </c>
+      <c r="F21" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>97</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5</v>
+      </c>
+      <c r="D22" s="9">
+        <v>23</v>
+      </c>
+      <c r="E22" s="9">
+        <v>94</v>
+      </c>
+      <c r="F22" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1">
+        <v>18</v>
+      </c>
+      <c r="D23" s="9">
+        <v>24</v>
+      </c>
+      <c r="E23" s="9">
+        <v>90</v>
+      </c>
+      <c r="F23" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>96</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
+      <c r="D24" s="9">
+        <v>25</v>
+      </c>
+      <c r="E24" s="9">
+        <v>90</v>
+      </c>
+      <c r="F24" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>88</v>
+      </c>
+      <c r="C25" s="1">
+        <v>14</v>
+      </c>
+      <c r="D25" s="9">
+        <v>26</v>
+      </c>
+      <c r="E25" s="9">
+        <v>93</v>
+      </c>
+      <c r="F25" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>88</v>
+      </c>
+      <c r="C26" s="1">
+        <v>14</v>
+      </c>
+      <c r="D26" s="9">
+        <v>27</v>
+      </c>
+      <c r="E26" s="9">
+        <v>94</v>
+      </c>
+      <c r="F26" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>87</v>
+      </c>
+      <c r="C27" s="1">
+        <v>15</v>
+      </c>
+      <c r="D27" s="9">
+        <v>28</v>
+      </c>
+      <c r="E27" s="9">
+        <v>82</v>
+      </c>
+      <c r="F27" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>94</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+      <c r="D28" s="9">
+        <v>29</v>
+      </c>
+      <c r="E28" s="9">
+        <v>85</v>
+      </c>
+      <c r="F28" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1">
+        <v>20</v>
+      </c>
+      <c r="D29" s="9">
+        <v>30</v>
+      </c>
+      <c r="E29" s="9">
+        <v>94</v>
+      </c>
+      <c r="F29" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1">
+        <v>97</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5</v>
+      </c>
+      <c r="D30" s="9">
+        <v>31</v>
+      </c>
+      <c r="E30" s="9">
+        <v>91</v>
+      </c>
+      <c r="F30" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1">
+        <v>12</v>
+      </c>
+      <c r="D31" s="9">
+        <v>32</v>
+      </c>
+      <c r="E31" s="9">
+        <v>90</v>
+      </c>
+      <c r="F31" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1">
+        <v>11</v>
+      </c>
+      <c r="D32" s="9">
+        <v>33</v>
+      </c>
+      <c r="E32" s="9">
+        <v>91</v>
+      </c>
+      <c r="F32" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>93</v>
+      </c>
+      <c r="C33" s="1">
+        <v>9</v>
+      </c>
+      <c r="D33" s="9">
+        <v>34</v>
+      </c>
+      <c r="E33" s="9">
+        <v>92</v>
+      </c>
+      <c r="F33" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1">
+        <v>96</v>
+      </c>
+      <c r="C34" s="1">
+        <v>6</v>
+      </c>
+      <c r="D34" s="9">
+        <v>35</v>
+      </c>
+      <c r="E34" s="9">
+        <v>98</v>
+      </c>
+      <c r="F34" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1">
+        <v>82</v>
+      </c>
+      <c r="C35" s="1">
+        <v>20</v>
+      </c>
+      <c r="D35" s="9">
+        <v>36</v>
+      </c>
+      <c r="E35" s="9">
+        <v>81</v>
+      </c>
+      <c r="F35" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>37</v>
+      </c>
+      <c r="B36" s="1">
+        <v>97</v>
+      </c>
+      <c r="C36" s="1">
+        <v>5</v>
+      </c>
+      <c r="D36" s="9">
+        <v>37</v>
+      </c>
+      <c r="E36" s="9">
+        <v>98</v>
+      </c>
+      <c r="F36" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1">
+        <v>94</v>
+      </c>
+      <c r="C37" s="1">
+        <v>8</v>
+      </c>
+      <c r="D37" s="9">
+        <v>38</v>
+      </c>
+      <c r="E37" s="9">
+        <v>99</v>
+      </c>
+      <c r="F37" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>39</v>
+      </c>
+      <c r="B38" s="1">
+        <v>99</v>
+      </c>
+      <c r="C38" s="1">
         <v>3</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="D38" s="9">
+        <v>39</v>
+      </c>
+      <c r="E38" s="9">
+        <v>99</v>
+      </c>
+      <c r="F38" s="9">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>40</v>
+      </c>
+      <c r="B39" s="1">
+        <v>97</v>
+      </c>
+      <c r="C39" s="1">
+        <v>5</v>
+      </c>
+      <c r="D39" s="9">
+        <v>40</v>
+      </c>
+      <c r="E39" s="9">
+        <v>98</v>
+      </c>
+      <c r="F39" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>41</v>
+      </c>
+      <c r="B40" s="1">
+        <v>98</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="9">
+        <v>41</v>
+      </c>
+      <c r="E40" s="9">
+        <v>100</v>
+      </c>
+      <c r="F40" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1">
+        <v>11</v>
+      </c>
+      <c r="D41" s="9">
+        <v>42</v>
+      </c>
+      <c r="E41" s="9">
+        <v>95</v>
+      </c>
+      <c r="F41" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43</v>
+      </c>
+      <c r="B42" s="1">
+        <v>88</v>
+      </c>
+      <c r="C42" s="1">
+        <v>14</v>
+      </c>
+      <c r="D42" s="9">
+        <v>44</v>
+      </c>
+      <c r="E42" s="9">
+        <v>89</v>
+      </c>
+      <c r="F42" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45</v>
+      </c>
+      <c r="B43" s="1">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="9">
+        <v>45</v>
+      </c>
+      <c r="E43" s="9">
+        <v>100</v>
+      </c>
+      <c r="F43" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>46</v>
+      </c>
+      <c r="B44" s="1">
+        <v>88</v>
+      </c>
+      <c r="C44" s="1">
+        <v>14</v>
+      </c>
+      <c r="D44" s="9">
+        <v>46</v>
+      </c>
+      <c r="E44" s="9">
+        <v>88</v>
+      </c>
+      <c r="F44" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>47</v>
+      </c>
+      <c r="B45" s="1">
+        <v>92</v>
+      </c>
+      <c r="C45" s="1">
+        <v>10</v>
+      </c>
+      <c r="D45" s="9">
+        <v>47</v>
+      </c>
+      <c r="E45" s="9">
+        <v>91</v>
+      </c>
+      <c r="F45" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>49</v>
+      </c>
+      <c r="B46" s="1">
+        <v>99</v>
+      </c>
+      <c r="C46" s="1">
+        <v>3</v>
+      </c>
+      <c r="D46" s="9">
+        <v>48</v>
+      </c>
+      <c r="E46" s="9">
+        <v>97</v>
+      </c>
+      <c r="F46" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>50</v>
+      </c>
+      <c r="B47" s="1">
+        <v>77</v>
+      </c>
+      <c r="C47" s="1">
+        <v>25</v>
+      </c>
+      <c r="D47" s="9">
+        <v>49</v>
+      </c>
+      <c r="E47" s="9">
+        <v>99</v>
+      </c>
+      <c r="F47" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>51</v>
+      </c>
+      <c r="B48" s="1">
+        <v>94</v>
+      </c>
+      <c r="C48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48" s="9">
+        <v>50</v>
+      </c>
+      <c r="E48" s="9">
+        <v>75</v>
+      </c>
+      <c r="F48" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>52</v>
+      </c>
+      <c r="B49" s="1">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1">
+        <v>4</v>
+      </c>
+      <c r="D49" s="9">
+        <v>51</v>
+      </c>
+      <c r="E49" s="9">
+        <v>99</v>
+      </c>
+      <c r="F49" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>53</v>
+      </c>
+      <c r="B50" s="1">
+        <v>96</v>
+      </c>
+      <c r="C50" s="1">
+        <v>6</v>
+      </c>
+      <c r="D50" s="9">
+        <v>52</v>
+      </c>
+      <c r="E50" s="9">
+        <v>95</v>
+      </c>
+      <c r="F50" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>55</v>
+      </c>
+      <c r="B51" s="1">
+        <v>97</v>
+      </c>
+      <c r="C51" s="1">
+        <v>5</v>
+      </c>
+      <c r="D51" s="9">
+        <v>53</v>
+      </c>
+      <c r="E51" s="9">
+        <v>95</v>
+      </c>
+      <c r="F51" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>57</v>
+      </c>
+      <c r="B52" s="1">
+        <v>99</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" s="9">
+        <v>54</v>
+      </c>
+      <c r="E52" s="9">
+        <v>99</v>
+      </c>
+      <c r="F52" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>59</v>
+      </c>
+      <c r="B53" s="1">
+        <v>97</v>
+      </c>
+      <c r="C53" s="1">
+        <v>5</v>
+      </c>
+      <c r="D53" s="9">
+        <v>55</v>
+      </c>
+      <c r="E53" s="9">
+        <v>96</v>
+      </c>
+      <c r="F53" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>60</v>
+      </c>
+      <c r="B54" s="1">
+        <v>92</v>
+      </c>
+      <c r="C54" s="1">
+        <v>10</v>
+      </c>
+      <c r="D54" s="9">
         <v>56</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E54" s="9">
+        <v>97</v>
+      </c>
+      <c r="F54" s="9">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <f>A2</f>
-        <v>1</v>
-      </c>
-      <c r="L2" s="1">
-        <f>B2/SUM(B2:C2)</f>
-        <v>0.875</v>
-      </c>
-      <c r="M2" s="1">
-        <f>C2/SUM(B2:C2)</f>
-        <v>0.125</v>
-      </c>
-      <c r="N2" s="1">
-        <f>D2</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <f>SUM(L2:L11)/10</f>
-        <v>0.84375</v>
-      </c>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>61</v>
+      </c>
+      <c r="B55" s="1">
+        <v>93</v>
+      </c>
+      <c r="C55" s="1">
+        <v>9</v>
+      </c>
+      <c r="D55" s="9">
+        <v>57</v>
+      </c>
+      <c r="E55" s="9">
+        <v>98</v>
+      </c>
+      <c r="F55" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>62</v>
+      </c>
+      <c r="B56" s="1">
+        <v>100</v>
+      </c>
+      <c r="C56" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="D56" s="9">
+        <v>58</v>
+      </c>
+      <c r="E56" s="9">
+        <v>82</v>
+      </c>
+      <c r="F56" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>64</v>
+      </c>
+      <c r="B57" s="1">
+        <v>98</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4</v>
+      </c>
+      <c r="D57" s="9">
+        <v>59</v>
+      </c>
+      <c r="E57" s="9">
+        <v>94</v>
+      </c>
+      <c r="F57" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>65</v>
+      </c>
+      <c r="B58" s="1">
+        <v>91</v>
+      </c>
+      <c r="C58" s="1">
+        <v>11</v>
+      </c>
+      <c r="D58" s="9">
+        <v>61</v>
+      </c>
+      <c r="E58" s="9">
+        <v>92</v>
+      </c>
+      <c r="F58" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>66</v>
+      </c>
+      <c r="B59" s="1">
+        <v>95</v>
+      </c>
+      <c r="C59" s="1">
+        <v>7</v>
+      </c>
+      <c r="D59" s="9">
+        <v>62</v>
+      </c>
+      <c r="E59" s="9">
+        <v>101</v>
+      </c>
+      <c r="F59" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>67</v>
+      </c>
+      <c r="B60" s="1">
+        <v>95</v>
+      </c>
+      <c r="C60" s="1">
+        <v>7</v>
+      </c>
+      <c r="D60" s="9">
+        <v>63</v>
+      </c>
+      <c r="E60" s="9">
+        <v>84</v>
+      </c>
+      <c r="F60" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>68</v>
+      </c>
+      <c r="B61" s="1">
+        <v>94</v>
+      </c>
+      <c r="C61" s="1">
+        <v>8</v>
+      </c>
+      <c r="D61" s="9">
+        <v>64</v>
+      </c>
+      <c r="E61" s="9">
+        <v>97</v>
+      </c>
+      <c r="F61" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>69</v>
+      </c>
+      <c r="B62" s="1">
+        <v>82</v>
+      </c>
+      <c r="C62" s="1">
+        <v>20</v>
+      </c>
+      <c r="D62" s="9">
+        <v>65</v>
+      </c>
+      <c r="E62" s="9">
+        <v>95</v>
+      </c>
+      <c r="F62" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>70</v>
+      </c>
+      <c r="B63" s="1">
+        <v>97</v>
+      </c>
+      <c r="C63" s="1">
+        <v>5</v>
+      </c>
+      <c r="D63" s="9">
+        <v>66</v>
+      </c>
+      <c r="E63" s="9">
+        <v>94</v>
+      </c>
+      <c r="F63" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>71</v>
+      </c>
+      <c r="B64" s="1">
+        <v>93</v>
+      </c>
+      <c r="C64" s="1">
+        <v>9</v>
+      </c>
+      <c r="D64" s="9">
+        <v>67</v>
+      </c>
+      <c r="E64" s="9">
+        <v>97</v>
+      </c>
+      <c r="F64" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>74</v>
+      </c>
+      <c r="B65" s="1">
+        <v>93</v>
+      </c>
+      <c r="C65" s="1">
+        <v>9</v>
+      </c>
+      <c r="D65" s="9">
+        <v>68</v>
+      </c>
+      <c r="E65" s="9">
+        <v>91</v>
+      </c>
+      <c r="F65" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>76</v>
+      </c>
+      <c r="B66" s="1">
+        <v>84</v>
+      </c>
+      <c r="C66" s="1">
+        <v>18</v>
+      </c>
+      <c r="D66" s="9">
+        <v>69</v>
+      </c>
+      <c r="E66" s="9">
+        <v>80</v>
+      </c>
+      <c r="F66" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>78</v>
+      </c>
+      <c r="B67" s="1">
+        <v>81</v>
+      </c>
+      <c r="C67" s="1">
+        <v>21</v>
+      </c>
+      <c r="D67" s="9">
+        <v>70</v>
+      </c>
+      <c r="E67" s="9">
+        <v>94</v>
+      </c>
+      <c r="F67" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>79</v>
+      </c>
+      <c r="B68" s="1">
+        <v>98</v>
+      </c>
+      <c r="C68" s="1">
+        <v>4</v>
+      </c>
+      <c r="D68" s="9">
+        <v>71</v>
+      </c>
+      <c r="E68" s="9">
+        <v>90</v>
+      </c>
+      <c r="F68" s="9">
         <v>15</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K21" si="0">A3</f>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>80</v>
+      </c>
+      <c r="B69" s="1">
+        <v>91</v>
+      </c>
+      <c r="C69" s="1">
+        <v>11</v>
+      </c>
+      <c r="D69" s="9">
+        <v>72</v>
+      </c>
+      <c r="E69" s="9">
+        <v>80</v>
+      </c>
+      <c r="F69" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>81</v>
+      </c>
+      <c r="B70" s="1">
+        <v>97</v>
+      </c>
+      <c r="C70" s="1">
+        <v>5</v>
+      </c>
+      <c r="D70" s="9">
+        <v>73</v>
+      </c>
+      <c r="E70" s="9">
+        <v>74</v>
+      </c>
+      <c r="F70" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>82</v>
+      </c>
+      <c r="B71" s="1">
+        <v>96</v>
+      </c>
+      <c r="C71" s="1">
+        <v>6</v>
+      </c>
+      <c r="D71" s="9">
+        <v>74</v>
+      </c>
+      <c r="E71" s="9">
+        <v>93</v>
+      </c>
+      <c r="F71" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>83</v>
+      </c>
+      <c r="B72" s="1">
+        <v>90</v>
+      </c>
+      <c r="C72" s="1">
+        <v>12</v>
+      </c>
+      <c r="D72" s="9">
+        <v>75</v>
+      </c>
+      <c r="E72" s="9">
+        <v>91</v>
+      </c>
+      <c r="F72" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>84</v>
+      </c>
+      <c r="B73" s="1">
+        <v>76</v>
+      </c>
+      <c r="C73" s="1">
+        <v>26</v>
+      </c>
+      <c r="D73" s="9">
+        <v>76</v>
+      </c>
+      <c r="E73" s="9">
+        <v>87</v>
+      </c>
+      <c r="F73" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>85</v>
+      </c>
+      <c r="B74" s="1">
+        <v>100</v>
+      </c>
+      <c r="C74" s="1">
         <v>2</v>
       </c>
-      <c r="L3" s="1">
-        <f>B3/SUM(B3:C3)</f>
-        <v>0.765625</v>
-      </c>
-      <c r="M3" s="1">
-        <f t="shared" ref="M3:M21" si="1">C3/SUM(B3:C3)</f>
-        <v>0.234375</v>
-      </c>
-      <c r="N3" s="1">
-        <f t="shared" ref="N3:N11" si="2">D3</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>59</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="D74" s="9">
+        <v>77</v>
+      </c>
+      <c r="E74" s="9">
+        <v>98</v>
+      </c>
+      <c r="F74" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>86</v>
+      </c>
+      <c r="B75" s="1">
+        <v>96</v>
+      </c>
+      <c r="C75" s="1">
+        <v>6</v>
+      </c>
+      <c r="D75" s="9">
+        <v>78</v>
+      </c>
+      <c r="E75" s="9">
+        <v>79</v>
+      </c>
+      <c r="F75" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>88</v>
+      </c>
+      <c r="B76" s="1">
+        <v>96</v>
+      </c>
+      <c r="C76" s="1">
+        <v>6</v>
+      </c>
+      <c r="D76" s="9">
+        <v>79</v>
+      </c>
+      <c r="E76" s="9">
+        <v>95</v>
+      </c>
+      <c r="F76" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>90</v>
+      </c>
+      <c r="B77" s="1">
+        <v>94</v>
+      </c>
+      <c r="C77" s="1">
+        <v>8</v>
+      </c>
+      <c r="D77" s="9">
+        <v>80</v>
+      </c>
+      <c r="E77" s="9">
+        <v>89</v>
+      </c>
+      <c r="F77" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>91</v>
+      </c>
+      <c r="B78" s="1">
+        <v>83</v>
+      </c>
+      <c r="C78" s="1">
+        <v>19</v>
+      </c>
+      <c r="D78" s="9">
+        <v>81</v>
+      </c>
+      <c r="E78" s="9">
+        <v>101</v>
+      </c>
+      <c r="F78" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>92</v>
+      </c>
+      <c r="B79" s="1">
+        <v>95</v>
+      </c>
+      <c r="C79" s="1">
+        <v>7</v>
+      </c>
+      <c r="D79" s="9">
+        <v>82</v>
+      </c>
+      <c r="E79" s="9">
+        <v>95</v>
+      </c>
+      <c r="F79" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>93</v>
+      </c>
+      <c r="B80" s="1">
+        <v>88</v>
+      </c>
+      <c r="C80" s="1">
+        <v>14</v>
+      </c>
+      <c r="D80" s="9">
+        <v>83</v>
+      </c>
+      <c r="E80" s="9">
+        <v>89</v>
+      </c>
+      <c r="F80" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>94</v>
+      </c>
+      <c r="B81" s="1">
+        <v>95</v>
+      </c>
+      <c r="C81" s="1">
+        <v>7</v>
+      </c>
+      <c r="D81" s="9">
+        <v>84</v>
+      </c>
+      <c r="E81" s="9">
+        <v>77</v>
+      </c>
+      <c r="F81" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>95</v>
+      </c>
+      <c r="B82" s="1">
+        <v>94</v>
+      </c>
+      <c r="C82" s="1">
+        <v>8</v>
+      </c>
+      <c r="D82" s="9">
+        <v>86</v>
+      </c>
+      <c r="E82" s="9">
+        <v>95</v>
+      </c>
+      <c r="F82" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>96</v>
+      </c>
+      <c r="B83" s="1">
+        <v>73</v>
+      </c>
+      <c r="C83" s="1">
+        <v>29</v>
+      </c>
+      <c r="D83" s="9">
+        <v>87</v>
+      </c>
+      <c r="E83" s="9">
+        <v>92</v>
+      </c>
+      <c r="F83" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>97</v>
+      </c>
+      <c r="B84" s="1">
+        <v>97</v>
+      </c>
+      <c r="C84" s="1">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L4" s="1">
-        <f>B4/SUM(B4:C4)</f>
-        <v>0.921875</v>
-      </c>
-      <c r="M4" s="1">
-        <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="N4" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L5" s="1">
-        <f>B5/SUM(B5:C5)</f>
-        <v>0.90625</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" si="1"/>
-        <v>9.375E-2</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L6" s="1">
-        <f>B6/SUM(B6:C6)</f>
-        <v>0.75</v>
-      </c>
-      <c r="M6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L7" s="1">
-        <f>B7/SUM(B7:C7)</f>
-        <v>0.640625</v>
-      </c>
-      <c r="M7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.359375</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>59</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L8" s="1">
-        <f>B8/SUM(B8:C8)</f>
-        <v>0.921875</v>
-      </c>
-      <c r="M8" s="1">
-        <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="D84" s="9">
+        <v>88</v>
+      </c>
+      <c r="E84" s="9">
+        <v>95</v>
+      </c>
+      <c r="F84" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>98</v>
+      </c>
+      <c r="B85" s="1">
+        <v>83</v>
+      </c>
+      <c r="C85" s="1">
+        <v>19</v>
+      </c>
+      <c r="D85" s="9">
+        <v>89</v>
+      </c>
+      <c r="E85" s="9">
+        <v>84</v>
+      </c>
+      <c r="F85" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>99</v>
+      </c>
+      <c r="B86" s="1">
+        <v>93</v>
+      </c>
+      <c r="C86" s="1">
+        <v>9</v>
+      </c>
+      <c r="D86" s="9">
+        <v>90</v>
+      </c>
+      <c r="E86" s="9">
+        <v>90</v>
+      </c>
+      <c r="F86" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>100</v>
+      </c>
+      <c r="B87" s="1">
+        <v>75</v>
+      </c>
+      <c r="C87" s="1">
+        <v>27</v>
+      </c>
+      <c r="D87" s="9">
+        <v>91</v>
+      </c>
+      <c r="E87" s="9">
+        <v>81</v>
+      </c>
+      <c r="F87" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="9">
+        <v>92</v>
+      </c>
+      <c r="E88" s="9">
+        <v>91</v>
+      </c>
+      <c r="F88" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="9">
+        <v>93</v>
+      </c>
+      <c r="E89" s="9">
+        <v>85</v>
+      </c>
+      <c r="F89" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="9">
+        <v>94</v>
+      </c>
+      <c r="E90" s="9">
+        <v>93</v>
+      </c>
+      <c r="F90" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="9">
+        <v>95</v>
+      </c>
+      <c r="E91" s="9">
+        <v>91</v>
+      </c>
+      <c r="F91" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="9">
+        <v>96</v>
+      </c>
+      <c r="E92" s="9">
+        <v>71</v>
+      </c>
+      <c r="F92" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="9">
+        <v>97</v>
+      </c>
+      <c r="E93" s="9">
+        <v>97</v>
+      </c>
+      <c r="F93" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>62</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L9" s="1">
-        <f>B9/SUM(B9:C9)</f>
-        <v>0.96875</v>
-      </c>
-      <c r="M9" s="1">
-        <f t="shared" si="1"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>49</v>
-      </c>
-      <c r="C10" s="1">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L10" s="1">
-        <f>B10/SUM(B10:C10)</f>
-        <v>0.765625</v>
-      </c>
-      <c r="M10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.234375</v>
-      </c>
-      <c r="N10" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="9">
+        <v>98</v>
+      </c>
+      <c r="E94" s="9">
+        <v>80</v>
+      </c>
+      <c r="F94" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="9">
+        <v>99</v>
+      </c>
+      <c r="E95" s="9">
+        <v>95</v>
+      </c>
+      <c r="F95" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>59</v>
-      </c>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L11" s="1">
-        <f>B11/SUM(B11:C11)</f>
-        <v>0.921875</v>
-      </c>
-      <c r="M11" s="1">
-        <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
-        <v>58</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <f>B12/SUM(B12:C12)</f>
-        <v>0.87878787878787878</v>
-      </c>
-      <c r="M12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.12121212121212122</v>
-      </c>
-      <c r="N12" s="2">
-        <f>D12</f>
-        <v>1</v>
-      </c>
-      <c r="O12" s="5">
-        <f>SUM(L12:L21)/10</f>
-        <v>0.79242424242424236</v>
-      </c>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>46</v>
-      </c>
-      <c r="C13" s="2">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L13" s="2">
-        <f>B13/SUM(B13:C13)</f>
-        <v>0.69696969696969702</v>
-      </c>
-      <c r="M13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30303030303030304</v>
-      </c>
-      <c r="N13" s="2">
-        <f t="shared" ref="N13:N21" si="3">D13</f>
-        <v>1</v>
-      </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
-        <v>62</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L14" s="2">
-        <f>B14/SUM(B14:C14)</f>
-        <v>0.93939393939393945</v>
-      </c>
-      <c r="M14" s="2">
-        <f t="shared" si="1"/>
-        <v>6.0606060606060608E-2</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>4</v>
-      </c>
-      <c r="B15" s="2">
-        <v>53</v>
-      </c>
-      <c r="C15" s="2">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="K15" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L15" s="2">
-        <f>B15/SUM(B15:C15)</f>
-        <v>0.80303030303030298</v>
-      </c>
-      <c r="M15" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19696969696969696</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2">
-        <v>46</v>
-      </c>
-      <c r="C16" s="2">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L16" s="2">
-        <f>B16/SUM(B16:C16)</f>
-        <v>0.69696969696969702</v>
-      </c>
-      <c r="M16" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30303030303030304</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2">
-        <v>23</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L17" s="2">
-        <f>B17/SUM(B17:C17)</f>
-        <v>0.65151515151515149</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="1"/>
-        <v>0.34848484848484851</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2">
-        <v>57</v>
-      </c>
-      <c r="C18" s="2">
-        <v>9</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L18" s="2">
-        <f>B18/SUM(B18:C18)</f>
-        <v>0.86363636363636365</v>
-      </c>
-      <c r="M18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2">
-        <v>59</v>
-      </c>
-      <c r="C19" s="2">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L19" s="2">
-        <f>B19/SUM(B19:C19)</f>
-        <v>0.89393939393939392</v>
-      </c>
-      <c r="M19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.10606060606060606</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>9</v>
-      </c>
-      <c r="B20" s="2">
-        <v>46</v>
-      </c>
-      <c r="C20" s="2">
-        <v>20</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L20" s="2">
-        <f>B20/SUM(B20:C20)</f>
-        <v>0.69696969696969702</v>
-      </c>
-      <c r="M20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30303030303030304</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="5"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2">
-        <v>53</v>
-      </c>
-      <c r="C21" s="2">
-        <v>13</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="K21" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L21" s="2">
-        <f>B21/SUM(B21:C21)</f>
-        <v>0.80303030303030298</v>
-      </c>
-      <c r="M21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19696969696969696</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="6"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="9">
+        <v>100</v>
+      </c>
+      <c r="E96" s="9">
+        <v>78</v>
+      </c>
+      <c r="F96" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D21">
-    <sortCondition ref="D1:D21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
+    <sortCondition ref="D1:D205"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="O2:O11"/>
-    <mergeCell ref="O12:O21"/>
-    <mergeCell ref="P12:P21"/>
-    <mergeCell ref="P2:P11"/>
+  <mergeCells count="8">
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>